<commit_message>
Run initial job scrape and update README.md table
</commit_message>
<xml_diff>
--- a/daily_matches/job_matches_2026-02-20.xlsx
+++ b/daily_matches/job_matches_2026-02-20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,70 +473,1330 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AI Engineer (Sample)</t>
+          <t>Machine Learning Engineer</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>Breeze Airways</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mountain View, CA</t>
+          <t>Salt Lake City, UT, US USA</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>95</v>
+        <v>22.2</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Python, TensorFlow</t>
+          <t>Data Scientist, Machine Learning Engineer, RAG, PyTorch, XGBoost, LightGBM, AWS SageMaker, MLflow, FastAPI, Docker</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2c</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://careers.google.com</t>
+          <t>https://www.indeed.com/viewjob?jk=d767420f2a9716f8</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer (Sample)</t>
+          <t>Senior DevOps Engineer</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Amazon</t>
+          <t>ＡＮＧＥＬ</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Seattle, WA</t>
+          <t>Provo, UT, US USA</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>88</v>
+        <v>14.4</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>PyTorch, AWS</t>
+          <t>RAG, S3, EC2, Docker, Kubernetes, CI/CD, Jenkins, GitHub Actions, Terraform, Git</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>5h</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://amazon.jobs</t>
+          <t>https://www.indeed.com/viewjob?jk=823a1663055adb51</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Senior Software Development Engineer in Test (SDET)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ECP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Milwaukee, WI, US USA</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>RAG, Copilot, Docker, Kubernetes, CI/CD, Jenkins, GitHub Actions, Git, PostgreSQL, SQL</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=6f996a8327315e55</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Senior Software Development Engineer in Test (SDET)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ECP</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Chicago, IL, US USA</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>RAG, Copilot, Docker, Kubernetes, CI/CD, Jenkins, GitHub Actions, Git, PostgreSQL, SQL</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=98807f643181f187</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Senior Software Development Engineer in Test (SDET)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ECP</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Denver, CO, US USA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>RAG, Copilot, Docker, Kubernetes, CI/CD, Jenkins, GitHub Actions, Git, PostgreSQL, SQL</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=a14f1745da350b3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sr Machine Learning Engineer</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Adobe</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>San Jose, CA, US USA</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer, Generative AI, RAG, TensorFlow, PyTorch, Docker, Kubernetes, CI/CD, Python, R</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=ac7c6c0c346a932e</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Solution Architect</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Engineers &amp; Constructors International</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Houston, TX, US USA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>RAG, Data Lake, Kubernetes, CI/CD, Terraform, Git, Kafka, NoSQL, Python, SQL</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=73d1e56137c584a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Senior Full-Stack Software Engineer, Web Acquisition</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SoFi</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>San Francisco, CA, US USA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>RAG, Docker, Kubernetes, Git, Snowflake, PostgreSQL, MySQL, SQL, R, Java</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=359277f28851c6e0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - Basking Ridge, NJ</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Optum</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Basking Ridge, NJ, US USA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>RAG, Docker, CI/CD, Jenkins, Git, Kafka, MySQL, SQL, R, Java</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=dd998da946c33fa1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Senior Cloud Platform Engineer</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Capgemini</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>New York, NY, US USA</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Generative AI, RAG, Gemini, S3, EC2, Jenkins, Git, PostgreSQL, Python, SQL</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=2f2b427895c42617</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Senior Cloud Engineer</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Capgemini</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>New York, NY, US USA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Generative AI, RAG, Gemini, S3, CI/CD, GitHub Actions, Git, Python, R, Scala</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=7f9c7c38b976d2a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Data Engineer III</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Dallas College</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Dallas, TX, US USA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Data Scientist, Copilot, Synapse, Dataflow, CI/CD, Power BI, Python, SQL, R, Scala</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=04110df5faabcfe4</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Sr. Software Engineer, Lennar.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Lennar</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Irving, TX, US USA</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>RAG, Docker, Kubernetes, CI/CD, GitHub Actions, Git, NoSQL, Python, SQL, R</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=eb71e199e97397c4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Palantir GenAI Software Engineer (Full Stack)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>AIG</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Atlanta, GA, US USA</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Generative AI, RAG, CI/CD, Terraform, NoSQL, Python, SQL, R, Java, Scala</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=78356f387cc4ade5</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Austin, TX, US USA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=a8d19f8507e3a736</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Boston, MA, US USA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=15898b3b54c26de5</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Portland, OR, US USA</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=63fe706a16e8cc8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Washington, DC, US USA</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=ee1bf89e4664819e</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Miami, FL, US USA</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=b68bcb4f6349f127</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Sacramento, CA, US USA</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=1aa9b3852d0d02f7</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Seattle, WA, US USA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=5af1c9659046e6e0</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>New York, NY, US USA</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=969ef223b94fac5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Dallas, TX, US USA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>10</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=b4198afb75c57326</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>San Diego, CA, US USA</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>10</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=72e2b445076de91d</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Jacksonville, FL, US USA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=1fbb3513083e45ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Atlanta, GA, US USA</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>10</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=29e54c91bf3bb986</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Houston, TX, US USA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>10</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=7bd2eb1d7c3e4527</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Salt Lake City, UT, US USA</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>10</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=eeda9da30f708f65</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>San Francisco, CA, US USA</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>10</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=b3af76475c4c6219</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Denver, CO, US USA</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>10</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=249b5da568dc438b</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Chicago, IL, US USA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>10</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=ea1f1dc0b072e3b7</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Los Angeles, CA, US USA</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>10</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=90e450af71abfe07</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - FrontEnd (Signup &amp; Activation)</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Scribd</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Phoenix, AZ, US USA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>10</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>RAG, Terraform, Kafka, MySQL, SQL, R, Java, Scala, A/B Testing</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=a7c591a6e758b68e</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Software Engineer Intern</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>San Francisco, CA, US USA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>10</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>RAG, PyTorch, OpenCV, Docker, Kubernetes, Git, Python, R, Scala</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=86551fb2ca368487</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Senior Microsoft Power Platform and Generative AI Developer</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>True Tandem</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Washington, DC, US USA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>10</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Generative AI, RAG, Copilot, S3, Git, Python, R, Java, Optimization</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=db232f94be813087</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Sr. Machine Learning Engineer, Adobe Firefly Services</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Adobe</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Seattle, WA, US USA</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>10</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer, Generative AI, RAG, PyTorch, Kubernetes, Python, R, Scala, Optimization</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=7d73949c9da5807e</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Software QA Tester</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ShipperHQ</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Austin, TX, US USA</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>10</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>RAG, Gemini, Copilot, Docker, CI/CD, Git, MySQL, SQL, R</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=1d5f38225865774b</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Data Engineer II</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Dallas College</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Dallas, TX, US USA</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>10</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Data Scientist, Copilot, Synapse, Dataflow, Power BI, Python, SQL, R, Scala</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/viewjob?jk=03c678b4a3e36747</t>
         </is>
       </c>
     </row>

</xml_diff>